<commit_message>
1. 添加CoinExchange算法 2. 添加BalancePartition算法递归实现 3. EditDistance算法测试用例
</commit_message>
<xml_diff>
--- a/Algorithms/Dp/Dp.xlsx
+++ b/Algorithms/Dp/Dp.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Knapsack" sheetId="1" r:id="rId1"/>
     <sheet name="LCS" sheetId="2" r:id="rId2"/>
     <sheet name="LIS" sheetId="3" r:id="rId3"/>
+    <sheet name="Coin Exchange" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
   <si>
     <t>P:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -217,6 +218,14 @@
   </si>
   <si>
     <t>dp[i,j] = s[i] == t[j] ? 1, return 对角线上1连续的最大次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coins:1,3,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>money:6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -249,7 +258,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -337,13 +346,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -400,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1983,7 +2010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -2160,4 +2187,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="8" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19">
+        <v>2</v>
+      </c>
+      <c r="E2" s="19">
+        <v>1</v>
+      </c>
+      <c r="F2" s="19">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19">
+        <v>2</v>
+      </c>
+      <c r="H2" s="19">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>